<commit_message>
23.4 and keep result open
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ausdeloitte-my.sharepoint.com/personal/hwang5_deloitte_com_au/Documents/Documents/UiPath/AOPS_UiPath/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://auspost-my.sharepoint.com/personal/he_wang27_auspost_com_au/Documents/Documents/UiPath/AOPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="309" documentId="13_ncr:1_{6C51D61D-883E-4984-84E9-1D36387C9001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F4CCE82-A639-4DED-B6AB-B8C833B7C910}"/>
+  <xr:revisionPtr revIDLastSave="370" documentId="13_ncr:1_{6C51D61D-883E-4984-84E9-1D36387C9001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A89F1D6A-7B0C-4DE0-A71D-5BBBFFE0D598}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Number Theory" sheetId="3" r:id="rId1"/>
     <sheet name="Counting &amp; Probability" sheetId="4" r:id="rId2"/>
-    <sheet name="Geometry" sheetId="5" r:id="rId3"/>
-    <sheet name="Algibra" sheetId="2" r:id="rId4"/>
-    <sheet name="Intermediate Algebra" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Geometry" sheetId="5" r:id="rId4"/>
+    <sheet name="Algibra" sheetId="2" r:id="rId5"/>
+    <sheet name="Intermediate Algebra" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Algibra!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Algibra!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Counting &amp; Probability'!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Geometry!$A$1:$J$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Intermediate Algebra'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Geometry!$A$1:$J$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Intermediate Algebra'!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Number Theory'!$A$1:$J$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1157,13 +1158,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1209,327 +1209,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="70">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="38">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1923,6 +1603,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2227,14 +1911,14 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2266,7 +1950,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -2297,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -2328,7 +2012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -2359,11 +2043,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5">
         <v>15</v>
       </c>
       <c r="C5">
@@ -2390,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -2421,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -2452,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -2483,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -2514,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -2545,11 +2229,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11">
         <v>14</v>
       </c>
       <c r="C11">
@@ -2576,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -2607,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -2638,11 +2322,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14">
         <v>15</v>
       </c>
       <c r="C14">
@@ -2669,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -2700,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -2731,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -2762,7 +2446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -2793,7 +2477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -2824,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -2855,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>128</v>
       </c>
@@ -2886,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -2917,7 +2601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>130</v>
       </c>
@@ -2948,7 +2632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -2979,7 +2663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -3010,7 +2694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>133</v>
       </c>
@@ -3041,7 +2725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -3072,7 +2756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -3103,7 +2787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -3134,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -3165,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>193</v>
       </c>
@@ -3173,7 +2857,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>194</v>
       </c>
@@ -3183,37 +2867,37 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J30" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="F2:F30">
+    <cfRule type="top10" dxfId="37" priority="1" percent="1" bottom="1" rank="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G30">
+    <cfRule type="top10" dxfId="36" priority="9" percent="1" rank="10"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H1 H31:H1048576">
-    <cfRule type="cellIs" dxfId="69" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1 J31:J1048576">
-    <cfRule type="cellIs" dxfId="67" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J30">
+    <cfRule type="top10" dxfId="32" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L25">
-    <cfRule type="cellIs" dxfId="66" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:L29">
-    <cfRule type="cellIs" dxfId="65" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
-    <cfRule type="top10" dxfId="64" priority="9" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J30">
-    <cfRule type="top10" dxfId="63" priority="2" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F30">
-    <cfRule type="top10" dxfId="62" priority="1" percent="1" bottom="1" rank="11"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3226,15 +2910,15 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" customWidth="1"/>
+    <col min="1" max="1" width="40.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3266,7 +2950,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -3297,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3328,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -3359,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -3390,7 +3074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -3421,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -3435,28 +3119,28 @@
         <v>17</v>
       </c>
       <c r="E7">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="F7">
-        <v>79.8</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="G7">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I7">
         <f>IF(E7&gt;30,IF( F7&gt;85,0,G7*5-E7), 30-E7)</f>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>144</v>
       </c>
@@ -3487,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>145</v>
       </c>
@@ -3522,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -3549,15 +3233,15 @@
         <v>26</v>
       </c>
       <c r="I10">
-        <f>IF(E10&gt;30,IF( F10&gt;85,0,G10*4-E10), 30-E10)</f>
-        <v>1</v>
+        <f>IF(E10&gt;30,IF( F10&gt;85,0,G10*5-E10), 30-E10)</f>
+        <v>19</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>147</v>
       </c>
@@ -3584,15 +3268,15 @@
         <v>19</v>
       </c>
       <c r="I11">
-        <f>IF(E11&gt;30,IF( F11&gt;85,0,G11*4-E11), 30-E11)</f>
-        <v>7</v>
+        <f>IF(E11&gt;30,IF( F11&gt;85,0,G11*5-E11), 30-E11)</f>
+        <v>31</v>
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -3623,7 +3307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -3637,28 +3321,28 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F13">
-        <v>90</v>
+        <v>93.8</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:I28" si="2">IF(E13&gt;30,IF( F13&gt;85,0,G13*5-E13), 30-E13)</f>
-        <v>10</v>
+        <f>IF(E13&gt;30,IF( F13&gt;85,,G13*5-E13), 30-E13)</f>
+        <v>0</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>150</v>
       </c>
@@ -3672,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F14">
         <v>100</v>
@@ -3682,18 +3366,18 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <f t="shared" ref="I13:I28" si="2">IF(E14&gt;30,IF( F14&gt;85,0,G14*5-E14), 30-E14)</f>
+        <v>5</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>151</v>
       </c>
@@ -3707,28 +3391,28 @@
         <v>11</v>
       </c>
       <c r="E15">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="F15">
-        <v>65.8</v>
+        <v>73.3</v>
       </c>
       <c r="G15">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="I15">
-        <f>IF(E15&gt;30,IF( F15&gt;85,0,G15*4-E15), 30-E15)</f>
-        <v>14</v>
+        <f>IF(E15&gt;30,IF( F15&gt;85,0,G15*5-E15), 30-E15)</f>
+        <v>25</v>
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>152</v>
       </c>
@@ -3742,28 +3426,28 @@
         <v>11</v>
       </c>
       <c r="E16">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="F16">
-        <v>71.099999999999994</v>
+        <v>76.7</v>
       </c>
       <c r="G16">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f>IF(E16&gt;30,IF( F16&gt;85,0,G16*5-E16), 30-E16)</f>
+        <v>10</v>
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>153</v>
       </c>
@@ -3798,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -3812,28 +3496,28 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F18">
-        <v>72.400000000000006</v>
+        <v>76.3</v>
       </c>
       <c r="G18">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>IF(E18&gt;30,IF( F18&gt;85,0,G18*5-E18), 30-E18)</f>
+        <v>7</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>155</v>
       </c>
@@ -3847,28 +3531,28 @@
         <v>20</v>
       </c>
       <c r="E19">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F19">
-        <v>63.8</v>
+        <v>65</v>
       </c>
       <c r="G19">
         <v>21</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I19">
-        <f>IF(E19&gt;30,IF( F19&gt;85,0,G19*4-E19), 30-E19)</f>
-        <v>26</v>
+        <f>IF(E19&gt;30,IF( F19&gt;85,0,G19*5-E19), 30-E19)</f>
+        <v>45</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>156</v>
       </c>
@@ -3882,28 +3566,28 @@
         <v>4</v>
       </c>
       <c r="E20">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F20">
-        <v>80</v>
+        <v>82.8</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>157</v>
       </c>
@@ -3930,7 +3614,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f>IF(E21&gt;30,IF( F21&gt;85,0,G21*5-E21), 30-E21)</f>
         <v>10</v>
       </c>
       <c r="J21">
@@ -3938,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>158</v>
       </c>
@@ -3973,7 +3657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>159</v>
       </c>
@@ -3987,28 +3671,28 @@
         <v>9</v>
       </c>
       <c r="E23">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F23">
-        <v>69.400000000000006</v>
+        <v>68.2</v>
       </c>
       <c r="G23">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I23">
+        <f>IF(E23&gt;30,IF( F23&gt;85,0,G23*5-E23), 30-E23)</f>
+        <v>21</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>160</v>
       </c>
@@ -4043,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>161</v>
       </c>
@@ -4078,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>162</v>
       </c>
@@ -4092,28 +3776,28 @@
         <v>3</v>
       </c>
       <c r="E26">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F26">
-        <v>84.2</v>
+        <v>85.7</v>
       </c>
       <c r="G26">
         <v>3</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -4148,7 +3832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -4183,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>197</v>
       </c>
@@ -4194,50 +3878,50 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="36" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="16" operator="lessThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E28">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="lessThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="35" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="15" operator="lessThan">
       <formula>85</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="34" priority="13" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J30">
-    <cfRule type="cellIs" dxfId="33" priority="10" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
+  <conditionalFormatting sqref="F2:F28">
+    <cfRule type="top10" dxfId="26" priority="1" percent="1" bottom="1" rank="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G28">
-    <cfRule type="top10" dxfId="32" priority="6" percent="1" rank="20"/>
-    <cfRule type="top10" dxfId="31" priority="8" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E28">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="lessThan">
-      <formula>25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J28">
-    <cfRule type="top10" dxfId="29" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="6" percent="1" rank="20"/>
+    <cfRule type="top10" dxfId="24" priority="8" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1 H31:H1048576">
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H28">
-    <cfRule type="top10" dxfId="26" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F28">
-    <cfRule type="top10" dxfId="13" priority="1" percent="1" bottom="1" rank="30"/>
+  <conditionalFormatting sqref="J1">
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J28">
+    <cfRule type="top10" dxfId="19" priority="5" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J30">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4245,6 +3929,491 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972F7013-DE23-408F-815F-19BB39AF553B}">
+  <dimension ref="B1:U9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:U9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>2023</v>
+      </c>
+      <c r="C1">
+        <v>2024</v>
+      </c>
+      <c r="D1">
+        <v>2025</v>
+      </c>
+      <c r="E1">
+        <v>2026</v>
+      </c>
+      <c r="F1">
+        <v>2027</v>
+      </c>
+      <c r="G1">
+        <v>2028</v>
+      </c>
+      <c r="H1">
+        <v>2029</v>
+      </c>
+      <c r="I1">
+        <v>2030</v>
+      </c>
+      <c r="J1">
+        <v>2031</v>
+      </c>
+      <c r="K1">
+        <v>2032</v>
+      </c>
+      <c r="L1">
+        <v>2033</v>
+      </c>
+      <c r="M1">
+        <v>2034</v>
+      </c>
+      <c r="N1">
+        <v>2035</v>
+      </c>
+      <c r="O1">
+        <v>2036</v>
+      </c>
+      <c r="P1">
+        <v>2037</v>
+      </c>
+      <c r="Q1">
+        <v>2038</v>
+      </c>
+      <c r="R1">
+        <v>2039</v>
+      </c>
+      <c r="S1">
+        <v>2040</v>
+      </c>
+      <c r="T1">
+        <v>2041</v>
+      </c>
+      <c r="U1">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>17700.900000000001</v>
+      </c>
+      <c r="C3">
+        <f>B3*1.05</f>
+        <v>18585.945000000003</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:U3" si="0">C3*1.05</f>
+        <v>19515.242250000003</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>20491.004362500003</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>21515.554580625005</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>22591.332309656256</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>23720.89892513907</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>24906.943871396026</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>26152.29106496583</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>27459.905618214121</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>28832.90089912483</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>30274.545944081074</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>31788.273241285129</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>33377.686903349386</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>35046.571248516855</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>36798.899810942698</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="0"/>
+        <v>38638.844801489831</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="0"/>
+        <v>40570.787041564327</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="0"/>
+        <v>42599.326393642543</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="0"/>
+        <v>44729.29271332467</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>26949.64</v>
+      </c>
+      <c r="C4">
+        <f>B4*1.02</f>
+        <v>27488.632799999999</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:U4" si="1">C4*1.02</f>
+        <v>28038.405456</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>28599.17356512</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>29171.157036422399</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>29754.580177150849</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>30349.671780693865</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>30956.665216307742</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>31575.798520633896</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>32207.314491046574</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>32851.460780867506</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>33508.489996484859</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>34178.659796414555</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>34862.232992342848</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>35559.477652189707</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>36270.667205233505</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="1"/>
+        <v>36996.080549338178</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="1"/>
+        <v>37736.002160324941</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>38490.722203531441</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="1"/>
+        <v>39260.536647602072</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>32897.93</v>
+      </c>
+      <c r="C5">
+        <f>B5*1.05</f>
+        <v>34542.826500000003</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:U5" si="2">C5*1.05</f>
+        <v>36269.967825000007</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>38083.46621625001</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>39987.639527062514</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>41987.021503415643</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>44086.37257858643</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>46290.691207515752</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>48605.225767891541</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>51035.487056286118</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>53587.261409100429</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>56266.624479555452</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>59079.955703533225</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="2"/>
+        <v>62033.953488709893</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>65135.65116314539</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>68392.433721302659</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="2"/>
+        <v>71812.055407367792</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="2"/>
+        <v>75402.658177736186</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="2"/>
+        <v>79172.791086622994</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="2"/>
+        <v>83131.430640954146</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <f>B3/B4</f>
+        <v>0.65681396857249308</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:U8" si="3">C3/C4</f>
+        <v>0.67613202647168413</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="3"/>
+        <v>0.69601826254438059</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>0.71648938791333305</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>0.73756260520490169</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>0.7592556230050459</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>0.78158667074048849</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>0.80457451399756175</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>0.8282384702916078</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>0.85259842530018448</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>0.87767484957371933</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>0.90348881573765227</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>0.93006201620052453</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="3"/>
+        <v>0.95741678138289277</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>0.98557609848238958</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>1.0145636307906951</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="3"/>
+        <v>1.0444037375786566</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="3"/>
+        <v>1.0751214945662642</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="3"/>
+        <v>1.1067427149946838</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="3"/>
+        <v>1.1392939713180568</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <f>B4/B5</f>
+        <v>0.81918953563339691</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:U9" si="4">C4/C5</f>
+        <v>0.79578412032958556</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="4"/>
+        <v>0.77304743117731167</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
+        <v>0.75096036171510272</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>0.72950435138038539</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>0.70866136991237438</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>0.68841390220059218</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>0.6687449335662895</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>0.64963793546439541</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>0.63107685159398419</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>0.61304608440558461</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>0.5955304819939965</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>0.57851532536559658</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>0.56198631606943661</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>0.54592956418173844</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="4"/>
+        <v>0.53033157663368879</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="4"/>
+        <v>0.51517924587272634</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="4"/>
+        <v>0.50045983884779122</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="4"/>
+        <v>0.48616098630928295</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="4"/>
+        <v>0.47227067241473203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
@@ -4253,12 +4422,12 @@
       <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4290,7 +4459,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>164</v>
       </c>
@@ -4321,7 +4490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -4352,7 +4521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -4383,7 +4552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -4414,7 +4583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -4445,7 +4614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -4476,7 +4645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>170</v>
       </c>
@@ -4507,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>171</v>
       </c>
@@ -4538,7 +4707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>172</v>
       </c>
@@ -4573,7 +4742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>173</v>
       </c>
@@ -4604,7 +4773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>174</v>
       </c>
@@ -4635,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>175</v>
       </c>
@@ -4666,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>176</v>
       </c>
@@ -4697,7 +4866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>177</v>
       </c>
@@ -4728,7 +4897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>178</v>
       </c>
@@ -4759,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>179</v>
       </c>
@@ -4790,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>180</v>
       </c>
@@ -4821,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -4852,7 +5021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -4887,7 +5056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>183</v>
       </c>
@@ -4922,7 +5091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>184</v>
       </c>
@@ -4957,7 +5126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -4992,7 +5161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>186</v>
       </c>
@@ -5027,7 +5196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>187</v>
       </c>
@@ -5062,7 +5231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>188</v>
       </c>
@@ -5097,7 +5266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -5132,7 +5301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>190</v>
       </c>
@@ -5167,7 +5336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>191</v>
       </c>
@@ -5202,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>192</v>
       </c>
@@ -5237,7 +5406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>194</v>
       </c>
@@ -5245,7 +5414,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>197</v>
       </c>
@@ -5255,50 +5424,40 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J30" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
-  <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="61" priority="15" operator="lessThan">
+  <conditionalFormatting sqref="E1:E30">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="lessThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="60" priority="14" operator="lessThan">
+  <conditionalFormatting sqref="F1:F30">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="lessThan">
       <formula>85</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G30">
+    <cfRule type="top10" dxfId="15" priority="1" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H30">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9 I11:I19">
-    <cfRule type="cellIs" dxfId="59" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H30">
-    <cfRule type="cellIs" dxfId="58" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="J2:J30">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J30">
-    <cfRule type="cellIs" dxfId="57" priority="4" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F30">
-    <cfRule type="cellIs" dxfId="56" priority="3" operator="lessThan">
-      <formula>85</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E30">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="lessThan">
-      <formula>20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
-    <cfRule type="top10" dxfId="54" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
@@ -5307,15 +5466,15 @@
       <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5347,7 +5506,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -5361,7 +5520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -5375,7 +5534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -5389,7 +5548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -5403,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -5417,7 +5576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -5431,7 +5590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -5445,7 +5604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -5459,7 +5618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -5473,7 +5632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -5487,7 +5646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -5501,7 +5660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -5515,7 +5674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -5529,7 +5688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -5543,7 +5702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -5557,7 +5716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -5571,7 +5730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -5585,7 +5744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -5599,7 +5758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -5613,7 +5772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -5627,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -5641,7 +5800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -5655,7 +5814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -5669,7 +5828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -5683,7 +5842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -5697,7 +5856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -5711,7 +5870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -5725,7 +5884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -5739,7 +5898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -5753,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -5767,7 +5926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -5781,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -5795,7 +5954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -5809,7 +5968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -5823,7 +5982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>92</v>
       </c>
@@ -5837,7 +5996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -5851,7 +6010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>93</v>
       </c>
@@ -5869,7 +6028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -5883,7 +6042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -5897,7 +6056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -5915,7 +6074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>95</v>
       </c>
@@ -5929,7 +6088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -5943,7 +6102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -5957,7 +6116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -5971,7 +6130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -5985,7 +6144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -5999,7 +6158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -6013,7 +6172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -6027,7 +6186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -6041,7 +6200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -6059,7 +6218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -6073,7 +6232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -6087,7 +6246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -6105,7 +6264,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>40</v>
       </c>
@@ -6119,7 +6278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>103</v>
       </c>
@@ -6133,7 +6292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -6147,7 +6306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -6161,7 +6320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>105</v>
       </c>
@@ -6175,7 +6334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>106</v>
       </c>
@@ -6189,7 +6348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>107</v>
       </c>
@@ -6203,7 +6362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>108</v>
       </c>
@@ -6221,7 +6380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>193</v>
       </c>
@@ -6229,7 +6388,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>194</v>
       </c>
@@ -6240,25 +6399,25 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="53" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="lessThan">
       <formula>85</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="49" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6267,23 +6426,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6315,7 +6474,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6350,7 +6509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -6385,7 +6544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -6420,7 +6579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -6455,7 +6614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -6490,7 +6649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -6525,7 +6684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -6560,7 +6719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -6595,7 +6754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -6630,7 +6789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -6665,7 +6824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -6700,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -6735,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -6770,7 +6929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -6805,7 +6964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -6840,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -6875,7 +7034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -6910,7 +7069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -6945,7 +7104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -6980,7 +7139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -7015,7 +7174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -7050,7 +7209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -7085,7 +7244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -7120,7 +7279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -7155,7 +7314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -7190,7 +7349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -7225,7 +7384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -7260,7 +7419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -7295,7 +7454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -7330,7 +7489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -7365,7 +7524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -7400,7 +7559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -7435,7 +7594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -7470,7 +7629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -7505,7 +7664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -7540,7 +7699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -7575,7 +7734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -7610,7 +7769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -7645,7 +7804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -7680,7 +7839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -7715,7 +7874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -7750,7 +7909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -7785,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -7820,7 +7979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -7855,7 +8014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -7890,7 +8049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -7925,7 +8084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -7960,7 +8119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -7995,7 +8154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -8030,7 +8189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -8065,7 +8224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -8100,7 +8259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -8135,7 +8294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -8170,7 +8329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -8205,7 +8364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -8240,7 +8399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -8278,29 +8437,29 @@
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="lessThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E57">
+    <cfRule type="top10" dxfId="5" priority="3" percent="1" bottom="1" rank="20"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="13" operator="lessThan">
       <formula>85</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J57">
-    <cfRule type="top10" dxfId="10" priority="5" percent="1" rank="5"/>
+  <conditionalFormatting sqref="F2:F57">
+    <cfRule type="top10" dxfId="3" priority="2" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G57">
-    <cfRule type="top10" dxfId="9" priority="4" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E57">
-    <cfRule type="top10" dxfId="8" priority="3" percent="1" bottom="1" rank="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F57">
-    <cfRule type="top10" dxfId="7" priority="2" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I57">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="30"/>
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J57">
+    <cfRule type="top10" dxfId="0" priority="5" percent="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>